<commit_message>
menu reorganization + calendar updates + detailed pdf schedule (not online yet) + jim's keynote title
</commit_message>
<xml_diff>
--- a/docs/schedule_full.xlsx
+++ b/docs/schedule_full.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14865" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14865" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="3" r:id="rId2"/>
+    <sheet name="Info" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Schedule!$A$2:$T$65</definedName>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>Day</t>
   </si>
@@ -135,10 +135,6 @@
 (14:00 - 15:30)</t>
   </si>
   <si>
-    <t>Tutorial: SDN, NFV and Their Role in 5G
-(14:00 - 15:30)</t>
-  </si>
-  <si>
     <t>Tutorial: Internet Measurements
 (14:00 - 15:30)</t>
   </si>
@@ -203,10 +199,6 @@
 (16:00 - 17:30)</t>
   </si>
   <si>
-    <t>Tutorial: SDN, NFV and Their Role in 5G
-(16:00 - 17:30)</t>
-  </si>
-  <si>
     <t>Tutorial: Internet Measurements
 (16:00 - 17:30)</t>
   </si>
@@ -219,10 +211,6 @@
 (19:00 - 21:00)</t>
   </si>
   <si>
-    <t>N2Women
-(20:00 - 22:30)</t>
-  </si>
-  <si>
     <t>Conference Banquet
 (19:00 - 23:30)</t>
   </si>
@@ -379,7 +367,17 @@
 (15:45 - 17:00)</t>
   </si>
   <si>
-    <t>Dimensions</t>
+    <t>Printing dimensions</t>
+  </si>
+  <si>
+    <t>N2Women
+(by invitation only)
+(20:00 - 22:30)</t>
+  </si>
+  <si>
+    <t>Award Dinner
+(by invitation only)
+(21:30 - 23:00)</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1179,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1221,33 +1219,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1257,113 +1232,14 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1371,6 +1247,168 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1383,6 +1421,21 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1401,14 +1454,26 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1436,9 +1501,20 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="45" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1454,6 +1530,9 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1469,6 +1548,18 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1484,6 +1575,9 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1508,6 +1602,9 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1532,16 +1629,28 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1550,93 +1659,16 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1645,7 +1677,11 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="100">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -2078,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="12.75"/>
@@ -2096,40 +2132,40 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="92" t="s">
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="92" t="s">
+      <c r="G2" s="116"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="92" t="s">
+      <c r="J2" s="116"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="92" t="s">
+      <c r="M2" s="116"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="94"/>
-      <c r="T2" s="138" t="s">
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18" thickTop="1" thickBot="1">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2144,17 +2180,17 @@
       <c r="E3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="99"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="122"/>
       <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2170,15 +2206,15 @@
       <c r="S3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="138" t="s">
+      <c r="T3" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A4" s="139">
+      <c r="A4" s="80">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="129"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -2196,13 +2232,13 @@
       <c r="Q4" s="19"/>
       <c r="R4" s="19"/>
       <c r="S4" s="20"/>
-      <c r="T4" s="139">
+      <c r="T4" s="80">
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A5" s="140"/>
-      <c r="B5" s="102"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="12"/>
       <c r="D5" s="16"/>
       <c r="E5" s="14"/>
@@ -2220,16 +2256,16 @@
       <c r="Q5" s="12"/>
       <c r="R5" s="11"/>
       <c r="S5" s="14"/>
-      <c r="T5" s="140"/>
+      <c r="T5" s="60"/>
     </row>
     <row r="6" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A6" s="139">
+      <c r="A6" s="80">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="131" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="16"/>
@@ -2237,1115 +2273,1111 @@
       <c r="F6" s="23"/>
       <c r="G6" s="12"/>
       <c r="H6" s="18"/>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="81" t="s">
+      <c r="J6" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="64" t="s">
+      <c r="K6" s="101"/>
+      <c r="L6" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="50" t="s">
+      <c r="M6" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="53" t="s">
+      <c r="N6" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="166" t="s">
-        <v>64</v>
-      </c>
-      <c r="P6" s="152" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="152" t="s">
-        <v>66</v>
+      <c r="O6" s="174" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" s="55" t="s">
+        <v>63</v>
       </c>
       <c r="R6" s="11"/>
       <c r="S6" s="14"/>
-      <c r="T6" s="139">
+      <c r="T6" s="80">
         <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A7" s="140"/>
-      <c r="B7" s="150"/>
-      <c r="C7" s="104"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="132"/>
       <c r="D7" s="12"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="111" t="s">
+      <c r="F7" s="144" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="175"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
       <c r="R7" s="12"/>
       <c r="S7" s="18"/>
-      <c r="T7" s="140"/>
+      <c r="T7" s="60"/>
     </row>
     <row r="8" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A8" s="139">
+      <c r="A8" s="80">
         <v>0.375</v>
       </c>
-      <c r="B8" s="150"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="36" t="s">
+      <c r="B8" s="127"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="112"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="136"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="156" t="s">
+      <c r="F8" s="145"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="175"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="177" t="s">
+        <v>64</v>
+      </c>
+      <c r="S8" s="178" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="80">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A9" s="60"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="175"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="179"/>
+      <c r="T9" s="60"/>
+    </row>
+    <row r="10" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A10" s="80">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B10" s="127"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="145"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="147"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="175"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="179"/>
+      <c r="T10" s="80">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A11" s="60"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="147"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="175"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="179"/>
+      <c r="T11" s="60"/>
+    </row>
+    <row r="12" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A12" s="80">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B12" s="127"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="175"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="179"/>
+      <c r="T12" s="80">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A13" s="60"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="176"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="180"/>
+      <c r="T13" s="60"/>
+    </row>
+    <row r="14" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A14" s="80">
+        <v>0.4375</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="111" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="101"/>
+      <c r="L14" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="36"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="106">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="13.5" thickBot="1">
+      <c r="A15" s="60"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="107"/>
+    </row>
+    <row r="16" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A16" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B16" s="143" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="111" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="101"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="O16" s="174" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q16" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="R16" s="177" t="s">
+        <v>68</v>
+      </c>
+      <c r="S16" s="178" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A17" s="60"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="175"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="179"/>
+      <c r="T17" s="60"/>
+    </row>
+    <row r="18" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A18" s="80">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B18" s="53"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="175"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="179"/>
+      <c r="T18" s="80">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A19" s="60"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="175"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="179"/>
+      <c r="T19" s="60"/>
+    </row>
+    <row r="20" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A20" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="175"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="179"/>
+      <c r="T20" s="80">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A21" s="60"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="112" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="33"/>
+      <c r="K21" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="109" t="s">
+        <v>42</v>
+      </c>
+      <c r="M21" s="36"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="176"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="180"/>
+      <c r="T21" s="60"/>
+    </row>
+    <row r="22" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A22" s="80">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B22" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="135"/>
+      <c r="D22" s="135"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="124" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="93"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="109" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="106">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A23" s="60"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="93"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="107"/>
+    </row>
+    <row r="24" spans="1:20" ht="12" customHeight="1" thickTop="1">
+      <c r="A24" s="80">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B24" s="137"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="93"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="106">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="12" customHeight="1" thickBot="1">
+      <c r="A25" s="60"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="91"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="114"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="107"/>
+    </row>
+    <row r="26" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A26" s="80">
+        <v>0.5625</v>
+      </c>
+      <c r="B26" s="137"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="91"/>
+      <c r="I26" s="99" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="M26" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="N26" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="106">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="13.5" thickBot="1">
+      <c r="A27" s="60"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="107"/>
+    </row>
+    <row r="28" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A28" s="80">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="47"/>
+      <c r="F28" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="63"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="174" t="s">
+        <v>84</v>
+      </c>
+      <c r="P28" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q28" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="R28" s="177" t="s">
+        <v>81</v>
+      </c>
+      <c r="S28" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="S8" s="157" t="s">
-        <v>68</v>
-      </c>
-      <c r="T8" s="139">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A9" s="140"/>
-      <c r="B9" s="150"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="136"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="140"/>
-    </row>
-    <row r="10" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A10" s="139">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="B10" s="150"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="136"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="139">
-        <v>0.39583333333333331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A11" s="140"/>
-      <c r="B11" s="150"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="113"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="136"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="140"/>
-    </row>
-    <row r="12" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A12" s="139">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B12" s="150"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="136"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="139">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A13" s="140"/>
-      <c r="B13" s="151"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="137"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="140"/>
-    </row>
-    <row r="14" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A14" s="139">
-        <v>0.4375</v>
-      </c>
-      <c r="B14" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="88"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="154" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="153" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="82"/>
-      <c r="L14" s="76" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="76"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="76"/>
-      <c r="R14" s="76"/>
-      <c r="S14" s="76"/>
-      <c r="T14" s="145">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A15" s="140"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="146"/>
-    </row>
-    <row r="16" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A16" s="141">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="152" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="154" t="s">
+      <c r="T28" s="80">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A29" s="60"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="175"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="179"/>
+      <c r="T29" s="60"/>
+    </row>
+    <row r="30" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A30" s="80">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B30" s="53"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="175"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="179"/>
+      <c r="T30" s="80">
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A31" s="60"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="36"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31" s="36"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="175"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="179"/>
+      <c r="T31" s="60"/>
+    </row>
+    <row r="32" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A32" s="80">
+        <v>0.625</v>
+      </c>
+      <c r="B32" s="53"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="175"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="179"/>
+      <c r="T32" s="80">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A33" s="60"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="176"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="57"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="180"/>
+      <c r="T33" s="60"/>
+    </row>
+    <row r="34" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A34" s="80">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="106">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A35" s="60"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="L35" s="96" t="s">
+        <v>74</v>
+      </c>
+      <c r="M35" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="N35" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="O35" s="36"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="36"/>
+      <c r="R35" s="36"/>
+      <c r="S35" s="36"/>
+      <c r="T35" s="107"/>
+    </row>
+    <row r="36" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A36" s="80">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B36" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="153" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="82"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="168" t="s">
-        <v>89</v>
-      </c>
-      <c r="M16" s="163" t="s">
-        <v>90</v>
-      </c>
-      <c r="N16" s="164" t="s">
-        <v>91</v>
-      </c>
-      <c r="O16" s="166" t="s">
-        <v>74</v>
-      </c>
-      <c r="P16" s="152" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q16" s="152" t="s">
-        <v>72</v>
-      </c>
-      <c r="R16" s="156" t="s">
-        <v>71</v>
-      </c>
-      <c r="S16" s="157" t="s">
-        <v>69</v>
-      </c>
-      <c r="T16" s="141">
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A17" s="140"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="84"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="136"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="140"/>
-    </row>
-    <row r="18" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A18" s="139">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="136"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="139">
-        <v>0.47916666666666669</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A19" s="140"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="140"/>
-    </row>
-    <row r="20" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A20" s="139">
-        <v>0.5</v>
-      </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="136"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="139">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A21" s="140"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="149" t="s">
-        <v>43</v>
-      </c>
-      <c r="J21" s="88"/>
-      <c r="K21" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="L21" s="167" t="s">
-        <v>43</v>
-      </c>
-      <c r="M21" s="76"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="137"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="140"/>
-    </row>
-    <row r="22" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A22" s="139">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="B22" s="147" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="148" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="76"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="76"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="167" t="s">
-        <v>41</v>
-      </c>
-      <c r="P22" s="76"/>
-      <c r="Q22" s="76"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="76"/>
-      <c r="T22" s="145">
-        <v>0.52083333333333337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A23" s="140"/>
-      <c r="B23" s="108"/>
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="76"/>
-      <c r="S23" s="76"/>
-      <c r="T23" s="146"/>
-    </row>
-    <row r="24" spans="1:20" ht="12" customHeight="1" thickTop="1">
-      <c r="A24" s="139">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B24" s="108"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="76"/>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="76"/>
-      <c r="R24" s="76"/>
-      <c r="S24" s="76"/>
-      <c r="T24" s="145">
-        <v>0.54166666666666663</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="12" customHeight="1" thickBot="1">
-      <c r="A25" s="140"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="76"/>
-      <c r="P25" s="76"/>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="76"/>
-      <c r="S25" s="76"/>
-      <c r="T25" s="146"/>
-    </row>
-    <row r="26" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A26" s="139">
-        <v>0.5625</v>
-      </c>
-      <c r="B26" s="108"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="168" t="s">
-        <v>75</v>
-      </c>
-      <c r="M26" s="163" t="s">
-        <v>38</v>
-      </c>
-      <c r="N26" s="164" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="76"/>
-      <c r="S26" s="76"/>
-      <c r="T26" s="145">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A27" s="140"/>
-      <c r="B27" s="108"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="146"/>
-    </row>
-    <row r="28" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A28" s="139">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="48"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="54"/>
-      <c r="O28" s="166" t="s">
-        <v>87</v>
-      </c>
-      <c r="P28" s="152" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q28" s="152" t="s">
-        <v>85</v>
-      </c>
-      <c r="R28" s="156" t="s">
-        <v>84</v>
-      </c>
-      <c r="S28" s="157" t="s">
-        <v>70</v>
-      </c>
-      <c r="T28" s="139">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A29" s="140"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="136"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="140"/>
-    </row>
-    <row r="30" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A30" s="139">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="136"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="37"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="139">
-        <v>0.60416666666666663</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A31" s="140"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="162" t="s">
+      <c r="C36" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="47"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="91"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="174" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="76"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="167" t="s">
-        <v>76</v>
-      </c>
-      <c r="M31" s="76"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="136"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="37"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="140"/>
-    </row>
-    <row r="32" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A32" s="139">
-        <v>0.625</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="136"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="139">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A33" s="140"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="162" t="s">
+      <c r="P36" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q36" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="R36" s="177" t="s">
+        <v>79</v>
+      </c>
+      <c r="S36" s="178" t="s">
+        <v>80</v>
+      </c>
+      <c r="T36" s="80">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A37" s="60"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="76"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="76"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="137"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="38"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="140"/>
-    </row>
-    <row r="34" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A34" s="139">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B34" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="76" t="s">
-        <v>11</v>
-      </c>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="76"/>
-      <c r="S34" s="76"/>
-      <c r="T34" s="145">
-        <v>0.64583333333333337</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A35" s="140"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="154" t="s">
-        <v>60</v>
-      </c>
-      <c r="J35" s="163" t="s">
-        <v>61</v>
-      </c>
-      <c r="K35" s="164" t="s">
-        <v>62</v>
-      </c>
-      <c r="L35" s="168" t="s">
-        <v>77</v>
-      </c>
-      <c r="M35" s="163" t="s">
-        <v>92</v>
-      </c>
-      <c r="N35" s="164" t="s">
-        <v>78</v>
-      </c>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
-      <c r="T35" s="146"/>
-    </row>
-    <row r="36" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A36" s="139">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B36" s="155" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="152" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="156" t="s">
+      <c r="I37" s="63"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="97"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="175"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="181"/>
+      <c r="T37" s="60"/>
+    </row>
+    <row r="38" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A38" s="81">
+        <v>0.6875</v>
+      </c>
+      <c r="B38" s="53"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="97"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="175"/>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="56"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="181"/>
+      <c r="T38" s="81">
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A39" s="82"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="175"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="181"/>
+      <c r="T39" s="82"/>
+    </row>
+    <row r="40" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A40" s="80">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B40" s="53"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" s="83"/>
+      <c r="N40" s="84"/>
+      <c r="O40" s="175"/>
+      <c r="P40" s="56"/>
+      <c r="Q40" s="56"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="181"/>
+      <c r="T40" s="80">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A41" s="60"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="85"/>
+      <c r="M41" s="85"/>
+      <c r="N41" s="86"/>
+      <c r="O41" s="176"/>
+      <c r="P41" s="57"/>
+      <c r="Q41" s="57"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="182"/>
+      <c r="T41" s="60"/>
+    </row>
+    <row r="42" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
+      <c r="A42" s="80">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="B42" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="157" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="75"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="166" t="s">
-        <v>79</v>
-      </c>
-      <c r="P36" s="152" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q36" s="152" t="s">
-        <v>81</v>
-      </c>
-      <c r="R36" s="156" t="s">
-        <v>82</v>
-      </c>
-      <c r="S36" s="157" t="s">
-        <v>83</v>
-      </c>
-      <c r="T36" s="139">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A37" s="140"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="154" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="163" t="s">
-        <v>58</v>
-      </c>
-      <c r="H37" s="164" t="s">
-        <v>59</v>
-      </c>
-      <c r="I37" s="48"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="65"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="54"/>
-      <c r="O37" s="136"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="37"/>
-      <c r="S37" s="169"/>
-      <c r="T37" s="140"/>
-    </row>
-    <row r="38" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A38" s="141">
-        <v>0.6875</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="65"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="54"/>
-      <c r="O38" s="136"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="37"/>
-      <c r="S38" s="169"/>
-      <c r="T38" s="141">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A39" s="142"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="136"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="37"/>
-      <c r="S39" s="169"/>
-      <c r="T39" s="142"/>
-    </row>
-    <row r="40" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A40" s="139">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" s="67"/>
-      <c r="N40" s="68"/>
-      <c r="O40" s="136"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="169"/>
-      <c r="T40" s="139">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A41" s="140"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
-      <c r="N41" s="70"/>
-      <c r="O41" s="137"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="170"/>
-      <c r="T41" s="140"/>
-    </row>
-    <row r="42" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A42" s="139">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="B42" s="158" t="s">
-        <v>51</v>
-      </c>
       <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="165" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="116"/>
-      <c r="K42" s="117"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="70"/>
+      <c r="I42" s="149" t="s">
+        <v>60</v>
+      </c>
+      <c r="J42" s="150"/>
+      <c r="K42" s="151"/>
+      <c r="L42" s="85"/>
+      <c r="M42" s="85"/>
+      <c r="N42" s="86"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
       <c r="R42" s="9"/>
       <c r="S42" s="13"/>
-      <c r="T42" s="139">
+      <c r="T42" s="80">
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A43" s="140"/>
+    <row r="43" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A43" s="60"/>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="10"/>
       <c r="G43" s="16"/>
       <c r="H43" s="14"/>
-      <c r="I43" s="118"/>
-      <c r="J43" s="119"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="71" t="s">
+      <c r="I43" s="152"/>
+      <c r="J43" s="153"/>
+      <c r="K43" s="154"/>
+      <c r="L43" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="M43" s="71"/>
-      <c r="N43" s="72"/>
+      <c r="M43" s="87"/>
+      <c r="N43" s="88"/>
       <c r="O43" s="11"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
       <c r="R43" s="11"/>
       <c r="S43" s="14"/>
-      <c r="T43" s="140"/>
+      <c r="T43" s="60"/>
     </row>
     <row r="44" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A44" s="139">
+      <c r="A44" s="80">
         <v>0.75</v>
       </c>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="47"/>
       <c r="F44" s="10"/>
       <c r="G44" s="16"/>
       <c r="H44" s="14"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="120"/>
-      <c r="L44" s="73"/>
-      <c r="M44" s="73"/>
-      <c r="N44" s="74"/>
+      <c r="I44" s="152"/>
+      <c r="J44" s="153"/>
+      <c r="K44" s="154"/>
+      <c r="L44" s="89"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="90"/>
       <c r="O44" s="11"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
       <c r="R44" s="11"/>
       <c r="S44" s="14"/>
-      <c r="T44" s="139">
+      <c r="T44" s="80">
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A45" s="140"/>
+    <row r="45" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A45" s="60"/>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="10"/>
       <c r="G45" s="16"/>
       <c r="H45" s="14"/>
-      <c r="I45" s="121"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="123"/>
+      <c r="I45" s="155"/>
+      <c r="J45" s="156"/>
+      <c r="K45" s="157"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="13"/>
@@ -3354,16 +3386,16 @@
       <c r="Q45" s="11"/>
       <c r="R45" s="11"/>
       <c r="S45" s="14"/>
-      <c r="T45" s="140"/>
+      <c r="T45" s="60"/>
     </row>
     <row r="46" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A46" s="139">
+      <c r="A46" s="80">
         <v>0.77083333333333337</v>
       </c>
       <c r="B46" s="44"/>
       <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="47"/>
       <c r="F46" s="10"/>
       <c r="G46" s="16"/>
       <c r="H46" s="14"/>
@@ -3378,16 +3410,16 @@
       <c r="Q46" s="11"/>
       <c r="R46" s="11"/>
       <c r="S46" s="14"/>
-      <c r="T46" s="139">
+      <c r="T46" s="80">
         <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A47" s="140"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="13"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="23"/>
       <c r="G47" s="12"/>
       <c r="H47" s="18"/>
@@ -3402,23 +3434,23 @@
       <c r="Q47" s="11"/>
       <c r="R47" s="11"/>
       <c r="S47" s="14"/>
-      <c r="T47" s="140"/>
+      <c r="T47" s="60"/>
     </row>
     <row r="48" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A48" s="139">
+      <c r="A48" s="80">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B48" s="158" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="132"/>
+      <c r="B48" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="183"/>
       <c r="D48" s="15"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="160" t="s">
-        <v>54</v>
-      </c>
-      <c r="G48" s="56"/>
-      <c r="H48" s="57"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="72"/>
+      <c r="H48" s="73"/>
       <c r="I48" s="10"/>
       <c r="J48" s="16"/>
       <c r="K48" s="14"/>
@@ -3430,19 +3462,19 @@
       <c r="Q48" s="16"/>
       <c r="R48" s="16"/>
       <c r="S48" s="14"/>
-      <c r="T48" s="139">
+      <c r="T48" s="80">
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A49" s="140"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="133"/>
+    <row r="49" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A49" s="60"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="185"/>
       <c r="D49" s="15"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="60"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="76"/>
       <c r="I49" s="23"/>
       <c r="J49" s="12"/>
       <c r="K49" s="18"/>
@@ -3454,24 +3486,24 @@
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
       <c r="S49" s="14"/>
-      <c r="T49" s="140"/>
+      <c r="T49" s="60"/>
     </row>
     <row r="50" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A50" s="143">
+      <c r="A50" s="59">
         <v>0.8125</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="133"/>
+      <c r="B50" s="184"/>
+      <c r="C50" s="185"/>
       <c r="D50" s="15"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="161" t="s">
-        <v>55</v>
-      </c>
-      <c r="J50" s="124"/>
-      <c r="K50" s="125"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="158" t="s">
+        <v>52</v>
+      </c>
+      <c r="J50" s="159"/>
+      <c r="K50" s="160"/>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
       <c r="N50" s="14"/>
@@ -3480,22 +3512,22 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" s="14"/>
-      <c r="T50" s="143">
+      <c r="T50" s="59">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A51" s="140"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="133"/>
+    <row r="51" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A51" s="60"/>
+      <c r="B51" s="184"/>
+      <c r="C51" s="185"/>
       <c r="D51" s="17"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="60"/>
-      <c r="I51" s="126"/>
-      <c r="J51" s="127"/>
-      <c r="K51" s="128"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="161"/>
+      <c r="J51" s="162"/>
+      <c r="K51" s="163"/>
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="14"/>
@@ -3504,24 +3536,24 @@
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
       <c r="S51" s="14"/>
-      <c r="T51" s="140"/>
+      <c r="T51" s="60"/>
     </row>
     <row r="52" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A52" s="143">
+      <c r="A52" s="59">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B52" s="41"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="159" t="s">
-        <v>53</v>
-      </c>
-      <c r="E52" s="40"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="126"/>
-      <c r="J52" s="127"/>
-      <c r="K52" s="128"/>
+      <c r="B52" s="184"/>
+      <c r="C52" s="185"/>
+      <c r="D52" s="169" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="170"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="161"/>
+      <c r="J52" s="162"/>
+      <c r="K52" s="163"/>
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
       <c r="N52" s="14"/>
@@ -3530,22 +3562,22 @@
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
       <c r="S52" s="14"/>
-      <c r="T52" s="143">
+      <c r="T52" s="59">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A53" s="140"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="134"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="59"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="126"/>
-      <c r="J53" s="127"/>
-      <c r="K53" s="128"/>
+    <row r="53" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A53" s="60"/>
+      <c r="B53" s="184"/>
+      <c r="C53" s="185"/>
+      <c r="D53" s="171"/>
+      <c r="E53" s="172"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="161"/>
+      <c r="J53" s="162"/>
+      <c r="K53" s="163"/>
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="14"/>
@@ -3554,22 +3586,22 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="14"/>
-      <c r="T53" s="140"/>
+      <c r="T53" s="60"/>
     </row>
     <row r="54" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A54" s="143">
+      <c r="A54" s="59">
         <v>0.85416666666666663</v>
       </c>
-      <c r="B54" s="41"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="134"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="60"/>
-      <c r="I54" s="126"/>
-      <c r="J54" s="127"/>
-      <c r="K54" s="128"/>
+      <c r="B54" s="184"/>
+      <c r="C54" s="185"/>
+      <c r="D54" s="171"/>
+      <c r="E54" s="172"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="161"/>
+      <c r="J54" s="162"/>
+      <c r="K54" s="163"/>
       <c r="L54" s="16"/>
       <c r="M54" s="16"/>
       <c r="N54" s="14"/>
@@ -3578,22 +3610,22 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
       <c r="S54" s="14"/>
-      <c r="T54" s="143">
+      <c r="T54" s="59">
         <v>0.85416666666666663</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A55" s="140"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="134"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="126"/>
-      <c r="J55" s="127"/>
-      <c r="K55" s="128"/>
+    <row r="55" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A55" s="60"/>
+      <c r="B55" s="186"/>
+      <c r="C55" s="187"/>
+      <c r="D55" s="171"/>
+      <c r="E55" s="172"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="161"/>
+      <c r="J55" s="162"/>
+      <c r="K55" s="163"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="14"/>
@@ -3602,22 +3634,22 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="16"/>
       <c r="S55" s="14"/>
-      <c r="T55" s="140"/>
+      <c r="T55" s="60"/>
     </row>
     <row r="56" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A56" s="143">
+      <c r="A56" s="59">
         <v>0.875</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="134"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="60"/>
-      <c r="I56" s="126"/>
-      <c r="J56" s="127"/>
-      <c r="K56" s="128"/>
+      <c r="D56" s="171"/>
+      <c r="E56" s="172"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="161"/>
+      <c r="J56" s="162"/>
+      <c r="K56" s="163"/>
       <c r="L56" s="16"/>
       <c r="M56" s="16"/>
       <c r="N56" s="14"/>
@@ -3626,22 +3658,24 @@
       <c r="Q56" s="16"/>
       <c r="R56" s="16"/>
       <c r="S56" s="14"/>
-      <c r="T56" s="143">
+      <c r="T56" s="59">
         <v>0.875</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A57" s="140"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="134"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="126"/>
-      <c r="J57" s="127"/>
-      <c r="K57" s="128"/>
+    <row r="57" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A57" s="60"/>
+      <c r="B57" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="40"/>
+      <c r="D57" s="167"/>
+      <c r="E57" s="172"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="161"/>
+      <c r="J57" s="162"/>
+      <c r="K57" s="163"/>
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="14"/>
@@ -3650,22 +3684,22 @@
       <c r="Q57" s="16"/>
       <c r="R57" s="16"/>
       <c r="S57" s="14"/>
-      <c r="T57" s="140"/>
+      <c r="T57" s="60"/>
     </row>
     <row r="58" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A58" s="143">
+      <c r="A58" s="59">
         <v>0.89583333333333337</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="134"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="126"/>
-      <c r="J58" s="127"/>
-      <c r="K58" s="128"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="167"/>
+      <c r="E58" s="172"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="76"/>
+      <c r="I58" s="161"/>
+      <c r="J58" s="162"/>
+      <c r="K58" s="163"/>
       <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="14"/>
@@ -3674,22 +3708,22 @@
       <c r="Q58" s="16"/>
       <c r="R58" s="16"/>
       <c r="S58" s="14"/>
-      <c r="T58" s="143">
+      <c r="T58" s="59">
         <v>0.89583333333333337</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A59" s="140"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="134"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="129"/>
-      <c r="J59" s="130"/>
-      <c r="K59" s="131"/>
+    <row r="59" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A59" s="60"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="167"/>
+      <c r="E59" s="172"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="164"/>
+      <c r="J59" s="165"/>
+      <c r="K59" s="166"/>
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="14"/>
@@ -3698,19 +3732,19 @@
       <c r="Q59" s="16"/>
       <c r="R59" s="16"/>
       <c r="S59" s="14"/>
-      <c r="T59" s="140"/>
+      <c r="T59" s="60"/>
     </row>
     <row r="60" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A60" s="143">
+      <c r="A60" s="59">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="134"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="60"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="167"/>
+      <c r="E60" s="172"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="76"/>
       <c r="I60" s="8"/>
       <c r="J60" s="9"/>
       <c r="K60" s="13"/>
@@ -3722,19 +3756,19 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="14"/>
-      <c r="T60" s="143">
+      <c r="T60" s="59">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A61" s="140"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="135"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="60"/>
+    <row r="61" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A61" s="60"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="168"/>
+      <c r="E61" s="173"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="76"/>
       <c r="I61" s="10"/>
       <c r="J61" s="16"/>
       <c r="K61" s="14"/>
@@ -3746,19 +3780,19 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="14"/>
-      <c r="T61" s="140"/>
+      <c r="T61" s="60"/>
     </row>
     <row r="62" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A62" s="143">
+      <c r="A62" s="59">
         <v>0.9375</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="16"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="43"/>
       <c r="D62" s="9"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="58"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="60"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="76"/>
       <c r="I62" s="10"/>
       <c r="J62" s="16"/>
       <c r="K62" s="14"/>
@@ -3770,19 +3804,19 @@
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
       <c r="S62" s="14"/>
-      <c r="T62" s="143">
+      <c r="T62" s="59">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A63" s="140"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="16"/>
+    <row r="63" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A63" s="60"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="46"/>
       <c r="D63" s="16"/>
       <c r="E63" s="14"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="60"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="75"/>
+      <c r="H63" s="76"/>
       <c r="I63" s="10"/>
       <c r="J63" s="16"/>
       <c r="K63" s="14"/>
@@ -3794,19 +3828,19 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="14"/>
-      <c r="T63" s="140"/>
+      <c r="T63" s="60"/>
     </row>
     <row r="64" spans="1:20" ht="12.95" customHeight="1" thickTop="1">
-      <c r="A64" s="144">
+      <c r="A64" s="61">
         <v>0.95833333333333337</v>
       </c>
-      <c r="B64" s="10"/>
+      <c r="B64" s="16"/>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
       <c r="E64" s="14"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="60"/>
+      <c r="F64" s="74"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="76"/>
       <c r="I64" s="10"/>
       <c r="J64" s="16"/>
       <c r="K64" s="14"/>
@@ -3818,19 +3852,19 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="14"/>
-      <c r="T64" s="144">
+      <c r="T64" s="61">
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A65" s="140"/>
-      <c r="B65" s="24"/>
+    <row r="65" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A65" s="60"/>
+      <c r="B65" s="25"/>
       <c r="C65" s="25"/>
       <c r="D65" s="25"/>
       <c r="E65" s="26"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="62"/>
-      <c r="H65" s="63"/>
+      <c r="F65" s="77"/>
+      <c r="G65" s="78"/>
+      <c r="H65" s="79"/>
       <c r="I65" s="24"/>
       <c r="J65" s="25"/>
       <c r="K65" s="26"/>
@@ -3842,9 +3876,9 @@
       <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
       <c r="S65" s="26"/>
-      <c r="T65" s="140"/>
-    </row>
-    <row r="66" spans="1:20" ht="13.5" thickTop="1">
+      <c r="T65" s="60"/>
+    </row>
+    <row r="66" spans="1:20" ht="13.5" customHeight="1" thickTop="1">
       <c r="A66" s="2"/>
       <c r="T66" s="2"/>
     </row>
@@ -3860,8 +3894,7 @@
     <mergeCell ref="R16:R21"/>
     <mergeCell ref="R8:R13"/>
     <mergeCell ref="S8:S13"/>
-    <mergeCell ref="O28:O33"/>
-    <mergeCell ref="P28:P33"/>
+    <mergeCell ref="O14:S15"/>
     <mergeCell ref="Q28:Q33"/>
     <mergeCell ref="R28:R33"/>
     <mergeCell ref="S28:S33"/>
@@ -3870,6 +3903,7 @@
     <mergeCell ref="Q36:Q41"/>
     <mergeCell ref="R36:R41"/>
     <mergeCell ref="S36:S41"/>
+    <mergeCell ref="O34:S35"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A48:A49"/>
@@ -3882,36 +3916,17 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B48:C55"/>
     <mergeCell ref="D52:E61"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B57:C63"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C6:C13"/>
+    <mergeCell ref="E8:E13"/>
     <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="B34:E35"/>
     <mergeCell ref="B22:E27"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="C16:C21"/>
     <mergeCell ref="D16:D21"/>
-    <mergeCell ref="E16:E21"/>
     <mergeCell ref="B14:E15"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="F7:H13"/>
-    <mergeCell ref="F16:F21"/>
-    <mergeCell ref="G16:H21"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="L35:L39"/>
-    <mergeCell ref="M35:M39"/>
-    <mergeCell ref="N35:N39"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A37"/>
@@ -3924,12 +3939,6 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="T46:T47"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="T10:T11"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:H2"/>
@@ -3948,34 +3957,36 @@
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="O14:S15"/>
-    <mergeCell ref="F33:H36"/>
-    <mergeCell ref="I31:K34"/>
-    <mergeCell ref="L31:N34"/>
-    <mergeCell ref="O34:S35"/>
-    <mergeCell ref="F22:H27"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="I14:I20"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="G28:G32"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="L21:N25"/>
-    <mergeCell ref="O22:S27"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="F14:H15"/>
     <mergeCell ref="J14:K20"/>
     <mergeCell ref="I26:I30"/>
     <mergeCell ref="J26:J30"/>
     <mergeCell ref="K26:K30"/>
     <mergeCell ref="I21:J25"/>
+    <mergeCell ref="T46:T47"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="F33:H36"/>
+    <mergeCell ref="I31:K34"/>
+    <mergeCell ref="L31:N34"/>
+    <mergeCell ref="F22:H27"/>
     <mergeCell ref="L6:L13"/>
     <mergeCell ref="M6:M13"/>
-    <mergeCell ref="L40:N42"/>
-    <mergeCell ref="L43:N44"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="F7:H13"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="G16:H21"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
     <mergeCell ref="I12:K13"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="K21:K25"/>
@@ -3985,14 +3996,8 @@
     <mergeCell ref="N16:N20"/>
     <mergeCell ref="I6:I11"/>
     <mergeCell ref="J6:K11"/>
-    <mergeCell ref="L26:L30"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="C36:C41"/>
-    <mergeCell ref="D36:D41"/>
-    <mergeCell ref="E36:E41"/>
-    <mergeCell ref="B42:E46"/>
-    <mergeCell ref="T60:T61"/>
+    <mergeCell ref="I14:I20"/>
+    <mergeCell ref="L21:N25"/>
     <mergeCell ref="T62:T63"/>
     <mergeCell ref="T64:T65"/>
     <mergeCell ref="F37:F41"/>
@@ -4010,6 +4015,35 @@
     <mergeCell ref="T40:T41"/>
     <mergeCell ref="T42:T43"/>
     <mergeCell ref="T44:T45"/>
+    <mergeCell ref="L40:N42"/>
+    <mergeCell ref="L43:N44"/>
+    <mergeCell ref="L35:L39"/>
+    <mergeCell ref="M35:M39"/>
+    <mergeCell ref="N35:N39"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="B34:D35"/>
+    <mergeCell ref="B42:D46"/>
+    <mergeCell ref="E28:E51"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="T60:T61"/>
+    <mergeCell ref="L26:L30"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="G28:G32"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="O22:S27"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="O28:O33"/>
+    <mergeCell ref="P28:P33"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="32767" scale="95" orientation="portrait" horizontalDpi="4000" verticalDpi="4000" r:id="rId1"/>
@@ -4025,15 +4059,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" s="171" t="s">
-        <v>93</v>
+      <c r="A2" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="B2">
         <v>715</v>

</xml_diff>